<commit_message>
change gitignore + things
</commit_message>
<xml_diff>
--- a/Lamia/DBASE/create/Base2_0_2.xlsx
+++ b/Lamia/DBASE/create/Base2_0_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="18" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="606">
   <si>
     <t>#DJAN</t>
   </si>
@@ -1789,6 +1789,102 @@
   </si>
   <si>
     <t>rue_complement</t>
+  </si>
+  <si>
+    <t>CD41</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Avant 1900 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1900-1920 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1921-1940 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1941-1950 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1951-1960 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1961-1970 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1971-1980 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1981-1990 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1991-1995 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1996-2000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2001-2005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2006-2010 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2011-2015 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2016-2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inconnue </t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>intervenant_1</t>
   </si>
 </sst>
 </file>
@@ -1847,9 +1943,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1863,7 +1968,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1884,6 +1989,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2191,8 +2298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3604,7 +3711,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8819,10 +8926,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8834,10 +8941,11 @@
     <col min="5" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="14" customWidth="1"/>
+    <col min="10" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8846,7 +8954,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8855,7 +8963,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -8864,7 +8972,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -8873,7 +8981,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>568</v>
       </c>
@@ -8881,8 +8989,11 @@
       <c r="F5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="14" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -8908,7 +9019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -8919,7 +9030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -8930,7 +9041,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -8944,7 +9055,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -8952,7 +9063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -8960,7 +9071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -8971,7 +9082,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>66</v>
       </c>
@@ -8979,7 +9090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>67</v>
       </c>
@@ -8987,7 +9098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>68</v>
       </c>
@@ -8995,7 +9106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -9006,7 +9117,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>66</v>
       </c>
@@ -9014,7 +9125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>67</v>
       </c>
@@ -9022,7 +9133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>68</v>
       </c>
@@ -9030,7 +9141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -9038,7 +9149,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -9046,7 +9157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>72</v>
       </c>
@@ -9057,7 +9168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>73</v>
       </c>
@@ -9065,7 +9176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>74</v>
       </c>
@@ -9073,7 +9184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>569</v>
       </c>
@@ -9081,7 +9192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>75</v>
       </c>
@@ -9089,7 +9200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>76</v>
       </c>
@@ -9099,92 +9210,210 @@
       <c r="F28" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>77</v>
       </c>
       <c r="G29" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>78</v>
       </c>
       <c r="G30" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>79</v>
       </c>
       <c r="G31" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>80</v>
       </c>
       <c r="G32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="I32" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="14" t="s">
+        <v>588</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>82</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>83</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>570</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B48" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>571</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B49" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>572</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>573</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B51" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>